<commit_message>
Update Excel to autonamically resolve registers
</commit_message>
<xml_diff>
--- a/AMREnergyMonitor/test/RFM69HCW_SPICommunication.xlsx
+++ b/AMREnergyMonitor/test/RFM69HCW_SPICommunication.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E9AFD46E-F07C-425F-A40C-CA7EEF2A68C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{69865577-366C-4771-9D0C-618A5AFF4497}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6090" yWindow="840" windowWidth="18195" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,9 +617,6 @@
     <t>0.100168250000000</t>
   </si>
   <si>
-    <t>------------ end of RH_RF69 -----------</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -705,6 +702,9 @@
   </si>
   <si>
     <t>setOpMode, read/write current mode</t>
+  </si>
+  <si>
+    <t>------------ end of RH_RF69::init -----------</t>
   </si>
 </sst>
 </file>
@@ -1779,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7469EA-CE2C-4277-A812-CB0611D1B417}">
   <dimension ref="A1:R109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3725,7 +3725,7 @@
         <v>0b10011111</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="J51" s="2"/>
       <c r="O51"/>
@@ -4697,7 +4697,7 @@
         <v>setSyncWords, burst write (len=2) 0x16,0x3a</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O77"/>
       <c r="P77"/>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="I81" s="2"/>
       <c r="J81" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O81"/>
       <c r="P81"/>
@@ -5890,20 +5890,20 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
         <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>76</v>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>77</v>
@@ -5919,7 +5919,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>78</v>
@@ -5927,10 +5927,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5938,12 +5938,12 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>84</v>
@@ -5951,18 +5951,18 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" t="s">
         <v>217</v>
-      </c>
-      <c r="B21" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -5970,15 +5970,15 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -5986,47 +5986,47 @@
         <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" t="s">
         <v>209</v>
-      </c>
-      <c r="B26" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" t="s">
         <v>215</v>
-      </c>
-      <c r="B29" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>